<commit_message>
Next levelup changes specifically for the classic mode
</commit_message>
<xml_diff>
--- a/docs/scoring_table.xlsx
+++ b/docs/scoring_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\screamingstrike\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>enemy_speed</t>
     <phoneticPr fontId="1"/>
@@ -63,6 +63,22 @@
   </si>
   <si>
     <t>hits</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>default_next_levelup_formula</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>next levelup defeats</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>classic_next_levelup_formula</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -393,14 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E7"/>
+  <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,6 +511,46 @@
         <v>9801</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B9">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <f>FLOOR(1+(B9*B9*0.25),1)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <f>FLOOR((2+B11)*0.7,1)</f>
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Levelup curb limitted to max 60 + showed collection unlocked ratio
</commit_message>
<xml_diff>
--- a/docs/scoring_table.xlsx
+++ b/docs/scoring_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\screamingstrike\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\screamingstrike\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -411,17 +411,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -438,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
         <v>500</v>
       </c>
@@ -453,7 +453,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
         <v>50</v>
       </c>
@@ -485,7 +485,7 @@
         <v>11250</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
         <v>11</v>
       </c>
@@ -511,7 +511,7 @@
         <v>9801</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -522,16 +522,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
         <v>16</v>
       </c>
       <c r="C9">
-        <f>FLOOR(1+(B9*B9*0.25),1)</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+        <f>MIN(60,FLOOR(1+(B9*B9*0.25),1))</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -542,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Add scoring  formula for burden mode
</commit_message>
<xml_diff>
--- a/docs/scoring_table.xlsx
+++ b/docs/scoring_table.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\screamingstrike\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98902976-DE5D-4CA8-98DD-A529B969BC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7470"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>enemy_speed</t>
     <phoneticPr fontId="1"/>
@@ -79,13 +80,21 @@
   </si>
   <si>
     <t>classic_next_levelup_formula</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BURDEN_MODE_Defeat_score=</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>negative effects</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,6 +144,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -151,10 +228,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -408,11 +485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -551,6 +628,38 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13">
+        <v>500</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>POWER(1.25,D13)*(1000-B13)*C13*C13/5</f>
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>